<commit_message>
Left to fix json request string. And replace solution of combinations
</commit_message>
<xml_diff>
--- a/Элементы СКС_для_Жени.xlsx
+++ b/Элементы СКС_для_Жени.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9636" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="ВОЛС" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="286">
   <si>
     <t>Кабель волоконно-оптический ОКЗ-СО -2/4 (2.0) Сп-8(2) "2,7кН</t>
   </si>
@@ -675,18 +675,6 @@
     <t>Межсетевой экран Cisco ASA5555-X</t>
   </si>
   <si>
-    <t>55547.42</t>
-  </si>
-  <si>
-    <t>14963.66</t>
-  </si>
-  <si>
-    <t>32858.88</t>
-  </si>
-  <si>
-    <t>34054.23</t>
-  </si>
-  <si>
     <t>ИБП</t>
   </si>
   <si>
@@ -726,45 +714,12 @@
     <t>Напряжение на входе, В</t>
   </si>
   <si>
-    <t>43.64</t>
-  </si>
-  <si>
     <t>Уровень шума, ДбА</t>
   </si>
   <si>
     <t>Эффективная мощность, ВА</t>
   </si>
   <si>
-    <t>16.36</t>
-  </si>
-  <si>
-    <t>21.36</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>9.09</t>
-  </si>
-  <si>
-    <t>11.36</t>
-  </si>
-  <si>
-    <t>10.77</t>
-  </si>
-  <si>
-    <t>12.7</t>
-  </si>
-  <si>
-    <t>11.34</t>
-  </si>
-  <si>
-    <t>12.27</t>
-  </si>
-  <si>
     <t>Количество портов коммутатора</t>
   </si>
   <si>
@@ -783,30 +738,6 @@
     <t>Поддержка Telnet</t>
   </si>
   <si>
-    <t>6.8</t>
-  </si>
-  <si>
-    <t>4.04</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>0.42</t>
-  </si>
-  <si>
-    <t>3.31</t>
-  </si>
-  <si>
     <t>Цена, руб.</t>
   </si>
   <si>
@@ -891,15 +822,9 @@
     <t>HPE 833870R-B21</t>
   </si>
   <si>
-    <t>2.2</t>
-  </si>
-  <si>
     <t>Частота, ГГЦ</t>
   </si>
   <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t>L2 кэш, Мб</t>
   </si>
   <si>
@@ -912,12 +837,6 @@
     <t>HPE 840370-B21</t>
   </si>
   <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>27.5</t>
-  </si>
-  <si>
     <t>Частота системной шины, МГц</t>
   </si>
   <si>
@@ -927,15 +846,6 @@
     <t>HPE 863446-B21</t>
   </si>
   <si>
-    <t>19.25</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>24.75</t>
-  </si>
-  <si>
     <t>HPE 869847-B21</t>
   </si>
   <si>
@@ -951,21 +861,12 @@
     <t>HPE 877619-421</t>
   </si>
   <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>8.25</t>
-  </si>
-  <si>
     <t>HPE 877620-421</t>
   </si>
   <si>
     <t>HPE 877622-421</t>
   </si>
   <si>
-    <t>13.75</t>
-  </si>
-  <si>
     <t>Цена, р/м</t>
   </si>
   <si>
@@ -988,21 +889,6 @@
   </si>
   <si>
     <t>Глубина</t>
-  </si>
-  <si>
-    <t>170528.88</t>
-  </si>
-  <si>
-    <t>161857.84</t>
-  </si>
-  <si>
-    <t>233304.86</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>0.3</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1085,17 +971,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1377,23 +1267,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1413,10 +1305,10 @@
         <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1331,7 @@
         <v>64.796000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1354,7 @@
         <v>39.659999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1485,7 +1377,7 @@
         <v>53.65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1508,7 +1400,7 @@
         <v>64.73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1531,7 +1423,7 @@
         <v>44.91</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1554,7 +1446,7 @@
         <v>95.64</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1577,7 +1469,7 @@
         <v>48.99</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1600,7 +1492,7 @@
         <v>91.56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +1515,7 @@
         <v>124.22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1646,32 +1538,32 @@
         <v>54.82</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="B13">
         <v>0.05</v>
@@ -1692,9 +1584,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1715,9 +1607,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1738,53 +1630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A31:J31"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1794,43 +1640,43 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H2" sqref="H2:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1852,14 +1698,14 @@
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>250</v>
+      <c r="H2" s="19">
+        <v>6.8</v>
       </c>
       <c r="I2" s="11">
         <v>123500</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>81</v>
       </c>
@@ -1888,7 +1734,7 @@
         <v>15274</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>82</v>
       </c>
@@ -1910,14 +1756,14 @@
       <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>236</v>
+      <c r="H4" s="14">
+        <v>0.5</v>
       </c>
       <c r="I4">
         <v>420</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>83</v>
       </c>
@@ -1939,14 +1785,14 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>257</v>
+      <c r="H5" s="14">
+        <v>3.31</v>
       </c>
       <c r="I5">
         <v>17150</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>84</v>
       </c>
@@ -1968,14 +1814,14 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>256</v>
+      <c r="H6" s="14">
+        <v>0.42</v>
       </c>
       <c r="I6">
         <v>1804</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>85</v>
       </c>
@@ -1997,14 +1843,14 @@
       <c r="G7" s="2">
         <v>0</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>255</v>
+      <c r="H7" s="14">
+        <v>1.5</v>
       </c>
       <c r="I7">
         <v>6620</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>86</v>
       </c>
@@ -2026,14 +1872,14 @@
       <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>254</v>
+      <c r="H8" s="14">
+        <v>2.9</v>
       </c>
       <c r="I8">
         <v>8270</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
@@ -2055,14 +1901,14 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>253</v>
+      <c r="H9" s="14">
+        <v>3.7</v>
       </c>
       <c r="I9">
         <v>20635</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>88</v>
       </c>
@@ -2084,14 +1930,14 @@
       <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>252</v>
+      <c r="H10" s="14">
+        <v>0.57999999999999996</v>
       </c>
       <c r="I10">
         <v>2650</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>89</v>
       </c>
@@ -2113,21 +1959,21 @@
       <c r="G11" s="2">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>251</v>
+      <c r="H11" s="14">
+        <v>4.04</v>
       </c>
       <c r="I11">
         <v>18120</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>43252</v>
       </c>
       <c r="D12">
@@ -2142,50 +1988,74 @@
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>236</v>
+      <c r="H12" s="14">
+        <v>0.5</v>
       </c>
       <c r="I12">
         <v>422</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C13" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D13" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E13" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F13" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="G13" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="I13" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="B14">
+        <v>0.1</v>
+      </c>
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>0.1</v>
+      </c>
+      <c r="I14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -2212,9 +2082,9 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2234,8 +2104,8 @@
       <c r="G16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>323</v>
+      <c r="H16" s="14">
+        <v>0.3</v>
       </c>
       <c r="I16" s="2">
         <v>400</v>
@@ -2251,58 +2121,58 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -2343,9 +2213,9 @@
         <v>3481</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -2384,9 +2254,9 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -2425,9 +2295,9 @@
         <v>5338</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="B5" s="12">
         <v>3</v>
@@ -2466,9 +2336,9 @@
         <v>2394</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="B6" s="12">
         <v>3</v>
@@ -2507,9 +2377,9 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -2548,9 +2418,9 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="B8" s="12">
         <v>3</v>
@@ -2589,9 +2459,9 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="B9" s="12">
         <v>3</v>
@@ -2630,9 +2500,9 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2671,9 +2541,9 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2712,55 +2582,91 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="F12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="G12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="H12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="I12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="J12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="K12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="L12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="M12" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -2799,9 +2705,9 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -2840,28 +2746,28 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
     </row>
   </sheetData>
@@ -2874,81 +2780,81 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="1" customWidth="1"/>
-    <col min="11" max="13" width="9.109375" style="1"/>
+    <col min="11" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="12" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="H1" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>286</v>
+      <c r="C2" s="18">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>288</v>
+      <c r="E2" s="14">
+        <v>2.5</v>
       </c>
       <c r="F2">
         <v>25</v>
@@ -2981,15 +2887,15 @@
         <v>101150</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>293</v>
+      <c r="C3" s="18">
+        <v>2.4</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -2997,8 +2903,8 @@
       <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>294</v>
+      <c r="F3" s="14">
+        <v>27.5</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -3028,15 +2934,15 @@
         <v>2181092</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>286</v>
+      <c r="C4" s="18">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D4">
         <v>14</v>
@@ -3044,8 +2950,8 @@
       <c r="E4">
         <v>14</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>298</v>
+      <c r="F4" s="14">
+        <v>19.25</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -3075,15 +2981,15 @@
         <v>646025</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>299</v>
+      <c r="C5" s="18">
+        <v>2.2999999999999998</v>
       </c>
       <c r="D5">
         <v>18</v>
@@ -3091,8 +2997,8 @@
       <c r="E5">
         <v>18</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>300</v>
+      <c r="F5" s="14">
+        <v>24.75</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -3122,15 +3028,15 @@
         <v>964490</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>301</v>
+        <v>271</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>293</v>
+      <c r="C6" s="18">
+        <v>2.4</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -3138,8 +3044,8 @@
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>294</v>
+      <c r="F6" s="14">
+        <v>27.5</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -3169,9 +3075,9 @@
         <v>2643775</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -3216,9 +3122,9 @@
         <v>76085</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -3263,15 +3169,15 @@
         <v>211779</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>306</v>
+      <c r="C9" s="18">
+        <v>1.7</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -3279,8 +3185,8 @@
       <c r="E9">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>307</v>
+      <c r="F9" s="14">
+        <v>8.25</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -3310,15 +3216,15 @@
         <v>141419</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>306</v>
+      <c r="C10" s="18">
+        <v>1.7</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -3357,15 +3263,15 @@
         <v>176726</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>286</v>
+      <c r="C11" s="18">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -3373,8 +3279,8 @@
       <c r="E11">
         <v>10</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>310</v>
+      <c r="F11" s="14">
+        <v>13.75</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -3404,61 +3310,103 @@
         <v>403328</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="H12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="I12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
@@ -3503,9 +3451,9 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -3559,20 +3507,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -3598,7 +3546,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3624,7 +3572,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -3650,7 +3598,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -3676,7 +3624,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -3702,7 +3650,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3728,7 +3676,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -3754,7 +3702,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -3780,7 +3728,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -3806,7 +3754,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3832,7 +3780,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3858,54 +3806,54 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3915,65 +3863,65 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
   </sheetData>
@@ -3989,21 +3937,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
@@ -4020,10 +3968,10 @@
         <v>107</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4043,7 +3991,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -4063,7 +4011,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -4083,7 +4031,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -4103,7 +4051,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -4123,7 +4071,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -4143,7 +4091,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -4163,29 +4111,29 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="B10" s="2">
         <v>0.3</v>
@@ -4203,9 +4151,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
@@ -4223,9 +4171,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -4243,7 +4191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -4252,7 +4200,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -4260,7 +4208,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -4268,7 +4216,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -4276,7 +4224,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -4284,7 +4232,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -4292,7 +4240,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -4300,7 +4248,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -4319,16 +4267,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>121</v>
       </c>
@@ -4351,13 +4299,13 @@
         <v>104</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>318</v>
+        <v>285</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -4386,7 +4334,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -4415,7 +4363,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -4444,7 +4392,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4473,7 +4421,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -4502,7 +4450,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -4531,7 +4479,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -4560,7 +4508,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -4589,7 +4537,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -4618,7 +4566,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -4647,7 +4595,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -4657,98 +4605,98 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -4759,34 +4707,34 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42"/>
     </row>
   </sheetData>
@@ -4799,28 +4747,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="11" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="11" width="13.7109375" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -4858,7 +4806,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -4896,7 +4844,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -4934,7 +4882,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -4972,7 +4920,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -5010,7 +4958,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -5048,7 +4996,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>157</v>
       </c>
@@ -5086,7 +5034,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -5124,47 +5072,47 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="G9" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="H9" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="I9" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="J9" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="K9" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="L9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>317</v>
+        <v>284</v>
       </c>
       <c r="B10">
         <v>0.05</v>
@@ -5200,9 +5148,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -5238,9 +5186,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5276,165 +5224,34 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A24:L24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>161</v>
       </c>
@@ -5466,7 +5283,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
@@ -5498,7 +5315,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -5530,7 +5347,7 @@
         <v>8.59</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -5562,7 +5379,7 @@
         <v>9.16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -5594,7 +5411,7 @@
         <v>13.17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="158.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -5626,7 +5443,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="171.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -5658,7 +5475,7 @@
         <v>175.8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -5690,7 +5507,7 @@
         <v>13.17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -5722,46 +5539,73 @@
         <v>20.62</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F10" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="G10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="H10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="I10" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="J10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="I11">
+        <v>0.1</v>
+      </c>
+      <c r="J11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5791,9 +5635,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -5823,111 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="C23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="C24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="E28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A27:J27"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5936,23 +5676,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>169</v>
       </c>
@@ -5993,7 +5733,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -6034,7 +5774,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
@@ -6075,7 +5815,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
@@ -6116,7 +5856,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -6157,7 +5897,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -6198,7 +5938,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
@@ -6239,7 +5979,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>62</v>
       </c>
@@ -6280,7 +6020,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>61</v>
       </c>
@@ -6321,7 +6061,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
@@ -6362,7 +6102,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
@@ -6403,7 +6143,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>65</v>
       </c>
@@ -6455,29 +6195,29 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>197</v>
       </c>
@@ -6527,7 +6267,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -6573,11 +6313,11 @@
       <c r="O2" s="1">
         <v>400</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="P2" s="17">
+        <v>170528.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>66</v>
       </c>
@@ -6623,11 +6363,11 @@
       <c r="O3" s="1">
         <v>400</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="P3" s="17">
+        <v>161857.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>67</v>
       </c>
@@ -6673,11 +6413,11 @@
       <c r="O4" s="1">
         <v>400</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="P4" s="17">
+        <v>233304.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>212</v>
       </c>
@@ -6723,11 +6463,11 @@
       <c r="O5" s="1">
         <v>450</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="16">
         <v>673016</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>213</v>
       </c>
@@ -6773,11 +6513,11 @@
       <c r="O6" s="1">
         <v>450</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="16">
         <v>934812</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>68</v>
       </c>
@@ -6823,11 +6563,11 @@
       <c r="O7" s="4">
         <v>350</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="P7" s="17">
+        <v>55547.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>69</v>
       </c>
@@ -6873,11 +6613,11 @@
       <c r="O8" s="4">
         <v>300</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="P8" s="18">
+        <v>14963.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>70</v>
       </c>
@@ -6923,11 +6663,11 @@
       <c r="O9" s="4">
         <v>350</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="P9" s="18">
+        <v>32858.879999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>71</v>
       </c>
@@ -6973,68 +6713,113 @@
       <c r="O10" s="4">
         <v>350</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="P10" s="18">
+        <v>34054.230000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="F11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="G11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="H11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="I11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="J11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="K11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="L11" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="N11" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="B12">
+        <v>0.1</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>0.1</v>
+      </c>
+      <c r="I12">
+        <v>0.1</v>
+      </c>
+      <c r="J12">
+        <v>0.1</v>
+      </c>
+      <c r="K12">
+        <v>0.1</v>
+      </c>
+      <c r="L12">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N12">
+        <v>0.1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B13">
         <v>5000</v>
@@ -7082,9 +6867,9 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -7132,7 +6917,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
     </row>
   </sheetData>
@@ -7146,61 +6931,61 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="1" max="1" width="22.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -7231,8 +7016,8 @@
       <c r="J2">
         <v>2</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>231</v>
+      <c r="K2" s="14">
+        <v>43.64</v>
       </c>
       <c r="L2">
         <v>47</v>
@@ -7244,7 +7029,7 @@
         <v>134719</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>72</v>
       </c>
@@ -7275,20 +7060,20 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
-        <v>234</v>
+      <c r="K3" s="19">
+        <v>16.36</v>
       </c>
       <c r="L3">
         <v>45</v>
       </c>
-      <c r="M3" s="15">
+      <c r="M3" s="14">
         <v>45</v>
       </c>
       <c r="N3">
         <v>123217</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>73</v>
       </c>
@@ -7319,8 +7104,8 @@
       <c r="J4">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>235</v>
+      <c r="K4" s="14">
+        <v>21.36</v>
       </c>
       <c r="L4">
         <v>45</v>
@@ -7332,7 +7117,7 @@
         <v>127453</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>74</v>
       </c>
@@ -7360,11 +7145,11 @@
       <c r="I5">
         <v>5</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>237</v>
+      <c r="J5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="14">
+        <v>10</v>
       </c>
       <c r="L5">
         <v>45</v>
@@ -7376,7 +7161,7 @@
         <v>98753</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>75</v>
       </c>
@@ -7404,11 +7189,11 @@
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>238</v>
+      <c r="J6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="14">
+        <v>9.09</v>
       </c>
       <c r="L6">
         <v>45</v>
@@ -7420,7 +7205,7 @@
         <v>105737</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>76</v>
       </c>
@@ -7451,8 +7236,8 @@
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>239</v>
+      <c r="K7" s="14">
+        <v>11.36</v>
       </c>
       <c r="L7">
         <v>38</v>
@@ -7464,7 +7249,7 @@
         <v>111546</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>77</v>
       </c>
@@ -7495,8 +7280,8 @@
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>240</v>
+      <c r="K8" s="14">
+        <v>10.77</v>
       </c>
       <c r="L8">
         <v>38</v>
@@ -7508,7 +7293,7 @@
         <v>110568</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>78</v>
       </c>
@@ -7539,8 +7324,8 @@
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>241</v>
+      <c r="K9" s="14">
+        <v>12.7</v>
       </c>
       <c r="L9">
         <v>38</v>
@@ -7552,7 +7337,7 @@
         <v>89076</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>79</v>
       </c>
@@ -7583,8 +7368,8 @@
       <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>242</v>
+      <c r="K10" s="14">
+        <v>11.34</v>
       </c>
       <c r="L10">
         <v>45</v>
@@ -7596,7 +7381,7 @@
         <v>96576</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>80</v>
       </c>
@@ -7627,8 +7412,8 @@
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>243</v>
+      <c r="K11" s="14">
+        <v>12.27</v>
       </c>
       <c r="L11">
         <v>45</v>
@@ -7640,58 +7425,97 @@
         <v>99456</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>314</v>
+        <v>281</v>
       </c>
       <c r="B12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="D12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="F12" t="s">
-        <v>315</v>
+        <v>282</v>
       </c>
       <c r="G12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="H12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="I12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="J12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="L12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="M12" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="N12" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="39.6" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="B13">
+        <v>0.1</v>
+      </c>
+      <c r="C13">
+        <v>0.1</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>0.1</v>
+      </c>
+      <c r="I13">
+        <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>0.1</v>
+      </c>
+      <c r="K13">
+        <v>0.1</v>
+      </c>
+      <c r="L13">
+        <v>0.1</v>
+      </c>
+      <c r="M13">
+        <v>0.1</v>
+      </c>
+      <c r="N13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="B14">
         <v>5000</v>
@@ -7733,9 +7557,9 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>313</v>
+        <v>280</v>
       </c>
       <c r="B15">
         <v>300</v>
@@ -7761,8 +7585,8 @@
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15" t="s">
-        <v>322</v>
+      <c r="J15" s="19">
+        <v>0.25</v>
       </c>
       <c r="K15">
         <v>5</v>

</xml_diff>

<commit_message>
Finished finding chain of alternatives with criterions sum lower than 80% or other set value. Only "Сплайс кассеты" doesn't work. Need to remake "Criterion for Сплайс кассеты.txt" and maybe something in excel file.
</commit_message>
<xml_diff>
--- a/Элементы СКС_для_Жени.xlsx
+++ b/Элементы СКС_для_Жени.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ВОЛС" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="259">
   <si>
     <t>Кабель волоконно-оптический ОКЗ-СО -2/4 (2.0) Сп-8(2) "2,7кН</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Монтаж</t>
   </si>
   <si>
-    <t>Шкаф или стойка 19"</t>
-  </si>
-  <si>
     <t>1U</t>
   </si>
   <si>
@@ -392,90 +389,18 @@
     <t>Количество адаптеров</t>
   </si>
   <si>
-    <t>200 рублей</t>
-  </si>
-  <si>
     <t>Сплайс кассеты</t>
   </si>
   <si>
-    <t xml:space="preserve">Количество КДЗС </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Материал </t>
-  </si>
-  <si>
     <t>АБС-пластик</t>
   </si>
   <si>
     <t>Черный</t>
   </si>
   <si>
-    <t>195х126х12</t>
-  </si>
-  <si>
-    <t>Габариты изделия, ШxВxГ , (мм)</t>
-  </si>
-  <si>
-    <t>100 рублей</t>
-  </si>
-  <si>
     <t>Шнуры ВОЛС</t>
   </si>
   <si>
-    <t>195х100х12</t>
-  </si>
-  <si>
-    <t>50 рублей</t>
-  </si>
-  <si>
-    <t>170х120х16</t>
-  </si>
-  <si>
-    <t>195х127х11</t>
-  </si>
-  <si>
-    <t>60 рублей</t>
-  </si>
-  <si>
-    <t>300 рублей</t>
-  </si>
-  <si>
-    <t>230х100х16</t>
-  </si>
-  <si>
-    <t>420 рублей</t>
-  </si>
-  <si>
-    <t>230х160х16</t>
-  </si>
-  <si>
-    <t>110х93х15</t>
-  </si>
-  <si>
-    <t>125 рублей</t>
-  </si>
-  <si>
-    <t>100х150х9</t>
-  </si>
-  <si>
-    <t>150 рублей</t>
-  </si>
-  <si>
-    <t>140 рублей</t>
-  </si>
-  <si>
-    <t>Белый</t>
-  </si>
-  <si>
-    <t>240х120х10</t>
-  </si>
-  <si>
-    <t>234х96х11</t>
-  </si>
-  <si>
-    <t>120 рублей</t>
-  </si>
-  <si>
     <t>Тип оптического волокна</t>
   </si>
   <si>
@@ -581,48 +506,15 @@
     <t>Ширина</t>
   </si>
   <si>
-    <t>111282 руб</t>
-  </si>
-  <si>
-    <t>170 651 руб</t>
-  </si>
-  <si>
     <t>USB, VGA, DVI-D</t>
   </si>
   <si>
     <t>PS/2, USB, VGA, DVI-D, HDMI, DisplayPort, Serial, Sun Legacy</t>
   </si>
   <si>
-    <t>244 723 руб</t>
-  </si>
-  <si>
-    <t>94 201 руб</t>
-  </si>
-  <si>
-    <t>143 162 руб</t>
-  </si>
-  <si>
     <t>USB, DVI-I</t>
   </si>
   <si>
-    <t>76 449 руб</t>
-  </si>
-  <si>
-    <t>86 756 руб</t>
-  </si>
-  <si>
-    <t>128 846 руб</t>
-  </si>
-  <si>
-    <t>137 436 руб</t>
-  </si>
-  <si>
-    <t>138 436 руб</t>
-  </si>
-  <si>
-    <t>148 889 руб</t>
-  </si>
-  <si>
     <t>Межсетевые экраны</t>
   </si>
   <si>
@@ -908,17 +800,23 @@
     <t>Хорошо</t>
   </si>
   <si>
-    <t>Плохо</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>Шкаф или стойка 19</t>
+  </si>
+  <si>
+    <t>Высота(U)</t>
+  </si>
+  <si>
+    <t>Количество КДЗС</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$RUB]\ #,##0.00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -944,12 +842,6 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -972,7 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1000,7 +892,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1012,14 +903,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1303,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1341,16 +1228,16 @@
         <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="H1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="I1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="J1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1675,39 +1562,39 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B13">
         <v>0.05</v>
@@ -1727,10 +1614,19 @@
       <c r="G13">
         <v>0.5</v>
       </c>
+      <c r="H13">
+        <v>0.5</v>
+      </c>
+      <c r="I13">
+        <v>0.5</v>
+      </c>
+      <c r="J13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1762,7 +1658,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1803,7 +1699,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="I14" sqref="I14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1818,37 +1714,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="66" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="J1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="K1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="L1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1873,7 +1769,7 @@
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="17">
         <v>6.8</v>
       </c>
       <c r="I2" s="11">
@@ -1949,7 +1845,7 @@
       <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>0.5</v>
       </c>
       <c r="I4">
@@ -1987,7 +1883,7 @@
       <c r="G5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>3.31</v>
       </c>
       <c r="I5">
@@ -2025,7 +1921,7 @@
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>0.42</v>
       </c>
       <c r="I6">
@@ -2063,7 +1959,7 @@
       <c r="G7" s="2">
         <v>0</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>1.5</v>
       </c>
       <c r="I7">
@@ -2101,7 +1997,7 @@
       <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>2.9</v>
       </c>
       <c r="I8">
@@ -2139,7 +2035,7 @@
       <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>3.7</v>
       </c>
       <c r="I9">
@@ -2177,7 +2073,7 @@
       <c r="G10" s="2">
         <v>0</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>0.57999999999999996</v>
       </c>
       <c r="I10">
@@ -2215,7 +2111,7 @@
       <c r="G11" s="2">
         <v>1</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>4.04</v>
       </c>
       <c r="I11">
@@ -2238,7 +2134,7 @@
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>43252</v>
       </c>
       <c r="D12">
@@ -2253,63 +2149,63 @@
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>0.5</v>
       </c>
       <c r="I12">
         <v>422</v>
       </c>
-      <c r="J12" s="14">
-        <v>3</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1</v>
-      </c>
-      <c r="L12" s="14">
+      <c r="J12" s="13">
+        <v>3</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1</v>
+      </c>
+      <c r="L12" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B13" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D13" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E13" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F13" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G13" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="I13" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B14">
         <v>0.1</v>
@@ -2333,12 +2229,21 @@
         <v>0.1</v>
       </c>
       <c r="I14">
+        <v>0.1</v>
+      </c>
+      <c r="J14">
+        <v>0.1</v>
+      </c>
+      <c r="K14">
+        <v>0.1</v>
+      </c>
+      <c r="L14">
         <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -2376,7 +2281,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2396,7 +2301,7 @@
       <c r="G16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <v>0.3</v>
       </c>
       <c r="I16" s="2">
@@ -2422,7 +2327,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="M13" sqref="M13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2440,49 +2345,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>237</v>
+        <v>201</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>238</v>
+        <v>202</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>240</v>
+        <v>204</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="N1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="O1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="P1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -2537,7 +2442,7 @@
     </row>
     <row r="3" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -2587,7 +2492,7 @@
     </row>
     <row r="4" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -2637,7 +2542,7 @@
     </row>
     <row r="5" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="B5" s="12">
         <v>3</v>
@@ -2687,7 +2592,7 @@
     </row>
     <row r="6" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="B6" s="12">
         <v>3</v>
@@ -2737,7 +2642,7 @@
     </row>
     <row r="7" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -2787,7 +2692,7 @@
     </row>
     <row r="8" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="B8" s="12">
         <v>3</v>
@@ -2837,7 +2742,7 @@
     </row>
     <row r="9" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="B9" s="12">
         <v>3</v>
@@ -2887,7 +2792,7 @@
     </row>
     <row r="10" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2937,7 +2842,7 @@
     </row>
     <row r="11" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2987,57 +2892,57 @@
     </row>
     <row r="12" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="F12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="G12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="H12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="I12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="J12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="K12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="L12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="M12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B13" s="1">
         <v>0.1</v>
@@ -3073,12 +2978,21 @@
         <v>0.1</v>
       </c>
       <c r="M13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P13" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -3128,7 +3042,7 @@
     </row>
     <row r="15" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -3210,7 +3124,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3231,71 +3145,71 @@
   <sheetData>
     <row r="1" spans="1:18" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="H1" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="P1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="Q1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="R1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>2.2000000000000002</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>2.5</v>
       </c>
       <c r="F2">
@@ -3340,12 +3254,12 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <v>2.4</v>
       </c>
       <c r="D3">
@@ -3354,7 +3268,7 @@
       <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>27.5</v>
       </c>
       <c r="G3" s="1">
@@ -3396,12 +3310,12 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>2.2000000000000002</v>
       </c>
       <c r="D4">
@@ -3410,7 +3324,7 @@
       <c r="E4">
         <v>14</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>19.25</v>
       </c>
       <c r="G4" s="1">
@@ -3452,12 +3366,12 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>2.2999999999999998</v>
       </c>
       <c r="D5">
@@ -3466,7 +3380,7 @@
       <c r="E5">
         <v>18</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>24.75</v>
       </c>
       <c r="G5" s="1">
@@ -3508,12 +3422,12 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>2.4</v>
       </c>
       <c r="D6">
@@ -3522,7 +3436,7 @@
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>27.5</v>
       </c>
       <c r="G6" s="1">
@@ -3564,7 +3478,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -3620,7 +3534,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -3676,12 +3590,12 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>1.7</v>
       </c>
       <c r="D9">
@@ -3690,7 +3604,7 @@
       <c r="E9">
         <v>6</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>8.25</v>
       </c>
       <c r="G9" s="1">
@@ -3732,12 +3646,12 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>1.7</v>
       </c>
       <c r="D10">
@@ -3788,12 +3702,12 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>2.2000000000000002</v>
       </c>
       <c r="D11">
@@ -3802,7 +3716,7 @@
       <c r="E11">
         <v>10</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>13.75</v>
       </c>
       <c r="G11" s="1">
@@ -3844,63 +3758,63 @@
     </row>
     <row r="12" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="H12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B13" s="1">
         <v>0.1</v>
@@ -3942,12 +3856,21 @@
         <v>0.1</v>
       </c>
       <c r="O13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R13" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
@@ -4003,7 +3926,7 @@
     </row>
     <row r="15" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -4064,17 +3987,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.44140625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -4092,28 +4015,28 @@
         <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>257</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="H1" t="s">
         <v>97</v>
       </c>
       <c r="I1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="J1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="K1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4124,10 +4047,10 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" t="s">
         <v>102</v>
-      </c>
-      <c r="D2" t="s">
-        <v>103</v>
       </c>
       <c r="E2">
         <v>482</v>
@@ -4142,13 +4065,13 @@
         <v>800</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="66" x14ac:dyDescent="0.25">
@@ -4156,13 +4079,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3">
         <v>183</v>
@@ -4177,13 +4100,13 @@
         <v>1500</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="66" x14ac:dyDescent="0.25">
@@ -4191,13 +4114,13 @@
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4">
         <v>390</v>
@@ -4212,13 +4135,13 @@
         <v>3100</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" x14ac:dyDescent="0.25">
@@ -4226,13 +4149,13 @@
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
         <v>111</v>
       </c>
-      <c r="C5" t="s">
-        <v>112</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5">
         <v>390</v>
@@ -4247,13 +4170,13 @@
         <v>2900</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4261,13 +4184,13 @@
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" t="s">
-        <v>103</v>
       </c>
       <c r="E6">
         <v>482</v>
@@ -4282,13 +4205,13 @@
         <v>1800</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4296,13 +4219,13 @@
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" t="s">
         <v>102</v>
-      </c>
-      <c r="D7" t="s">
-        <v>103</v>
       </c>
       <c r="E7">
         <v>482</v>
@@ -4317,13 +4240,13 @@
         <v>2700</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4331,13 +4254,13 @@
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" t="s">
         <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
       </c>
       <c r="E8">
         <v>482</v>
@@ -4352,13 +4275,13 @@
         <v>3500</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4366,13 +4289,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" t="s">
         <v>102</v>
-      </c>
-      <c r="D9" t="s">
-        <v>103</v>
       </c>
       <c r="E9">
         <v>482</v>
@@ -4387,13 +4310,13 @@
         <v>1700</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4401,13 +4324,13 @@
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D10" t="s">
         <v>102</v>
-      </c>
-      <c r="D10" t="s">
-        <v>103</v>
       </c>
       <c r="E10">
         <v>482</v>
@@ -4422,13 +4345,13 @@
         <v>2400</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4436,13 +4359,13 @@
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" t="s">
         <v>102</v>
-      </c>
-      <c r="D11" t="s">
-        <v>103</v>
       </c>
       <c r="E11">
         <v>482</v>
@@ -4457,142 +4380,16 @@
         <v>3100</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+        <v>253</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A31:H31"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4602,8 +4399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4620,31 +4417,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="G1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="H1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="I1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="66" x14ac:dyDescent="0.25">
@@ -4852,36 +4649,36 @@
     </row>
     <row r="9" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F9" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B10" s="2">
         <v>0.3</v>
@@ -4898,10 +4695,19 @@
       <c r="F10" s="2">
         <v>0.2</v>
       </c>
+      <c r="G10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
@@ -4930,7 +4736,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -5026,10 +4832,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5037,52 +4843,48 @@
     <col min="1" max="1" width="33.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>122</v>
+        <v>258</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>104</v>
+        <v>249</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>97</v>
+        <v>189</v>
+      </c>
+      <c r="I1" t="s">
+        <v>250</v>
       </c>
       <c r="J1" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="K1" t="s">
-        <v>287</v>
-      </c>
-      <c r="L1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -5090,37 +4892,34 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2">
+        <v>195</v>
+      </c>
+      <c r="F2">
         <v>126</v>
       </c>
-      <c r="F2">
-        <v>195</v>
-      </c>
       <c r="G2">
-        <v>126</v>
-      </c>
-      <c r="H2">
         <v>12</v>
       </c>
+      <c r="H2" s="2">
+        <v>100</v>
+      </c>
       <c r="I2" s="2" t="s">
-        <v>128</v>
+        <v>255</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -5128,37 +4927,34 @@
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
+      </c>
+      <c r="E3">
+        <v>195</v>
       </c>
       <c r="F3">
-        <v>195</v>
+        <v>127</v>
       </c>
       <c r="G3">
-        <v>127</v>
-      </c>
-      <c r="H3">
         <v>11</v>
       </c>
+      <c r="H3" s="2">
+        <v>60</v>
+      </c>
       <c r="I3" s="2" t="s">
-        <v>134</v>
+        <v>255</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -5166,37 +4962,34 @@
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>132</v>
+        <v>107</v>
+      </c>
+      <c r="E4">
+        <v>170</v>
       </c>
       <c r="F4">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="G4">
-        <v>120</v>
-      </c>
-      <c r="H4">
         <v>16</v>
       </c>
+      <c r="H4" s="2">
+        <v>200</v>
+      </c>
       <c r="I4" s="2" t="s">
-        <v>120</v>
+        <v>254</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5204,37 +4997,34 @@
         <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" t="s">
-        <v>136</v>
+        <v>107</v>
+      </c>
+      <c r="E5">
+        <v>230</v>
       </c>
       <c r="F5">
-        <v>230</v>
+        <v>100</v>
       </c>
       <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
         <v>16</v>
       </c>
+      <c r="H5" s="2">
+        <v>300</v>
+      </c>
       <c r="I5" s="2" t="s">
-        <v>135</v>
+        <v>255</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -5242,37 +5032,34 @@
         <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" t="s">
-        <v>138</v>
+        <v>107</v>
+      </c>
+      <c r="E6">
+        <v>230</v>
       </c>
       <c r="F6">
-        <v>230</v>
+        <v>160</v>
       </c>
       <c r="G6">
-        <v>160</v>
-      </c>
-      <c r="H6">
         <v>16</v>
       </c>
+      <c r="H6" s="2">
+        <v>420</v>
+      </c>
       <c r="I6" s="2" t="s">
-        <v>137</v>
+        <v>255</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -5280,37 +5067,34 @@
         <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
+      </c>
+      <c r="E7">
+        <v>195</v>
       </c>
       <c r="F7">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
         <v>12</v>
       </c>
+      <c r="H7" s="2">
+        <v>50</v>
+      </c>
       <c r="I7" s="2" t="s">
-        <v>131</v>
+        <v>254</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -5318,37 +5102,34 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>139</v>
+        <v>107</v>
+      </c>
+      <c r="E8">
+        <v>110</v>
       </c>
       <c r="F8">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G8">
-        <v>93</v>
-      </c>
-      <c r="H8">
         <v>15</v>
       </c>
+      <c r="H8" s="2">
+        <v>125</v>
+      </c>
       <c r="I8" s="2" t="s">
-        <v>140</v>
+        <v>255</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -5356,37 +5137,34 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>141</v>
+        <v>107</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2">
         <v>150</v>
       </c>
-      <c r="H9">
-        <v>9</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>142</v>
+        <v>254</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -5394,37 +5172,34 @@
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>145</v>
+        <v>107</v>
+      </c>
+      <c r="E10">
+        <v>240</v>
       </c>
       <c r="F10">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="G10">
-        <v>120</v>
-      </c>
-      <c r="H10">
         <v>10</v>
       </c>
+      <c r="H10" s="2">
+        <v>140</v>
+      </c>
       <c r="I10" s="2" t="s">
-        <v>143</v>
+        <v>254</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -5432,187 +5207,34 @@
         <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>146</v>
+        <v>107</v>
+      </c>
+      <c r="E11">
+        <v>234</v>
       </c>
       <c r="F11">
-        <v>234</v>
+        <v>96</v>
       </c>
       <c r="G11">
-        <v>96</v>
-      </c>
-      <c r="H11">
         <v>11</v>
       </c>
+      <c r="H11" s="2">
+        <v>120</v>
+      </c>
       <c r="I11" s="2" t="s">
-        <v>147</v>
+        <v>254</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42"/>
+        <v>255</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A31:H31"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5621,8 +5243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5644,49 +5266,49 @@
   <sheetData>
     <row r="1" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>97</v>
       </c>
       <c r="M1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="N1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="O1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="118.8" x14ac:dyDescent="0.25">
@@ -5926,7 +5548,7 @@
     </row>
     <row r="7" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -6020,54 +5642,54 @@
     </row>
     <row r="9" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G9" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="H9" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="I9" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="J9" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="K9" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="L9" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B10">
         <v>0.05</v>
@@ -6102,10 +5724,19 @@
       <c r="L10" s="2">
         <v>0.1</v>
       </c>
+      <c r="M10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -6152,7 +5783,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6206,8 +5837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6228,43 +5859,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="C1" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="G1" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="H1" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="I1" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>97</v>
       </c>
       <c r="K1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="L1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="M1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="79.2" x14ac:dyDescent="0.25">
@@ -6597,48 +6228,48 @@
     </row>
     <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F10" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="G10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="H10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I10" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="J10" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -6665,12 +6296,21 @@
         <v>0.1</v>
       </c>
       <c r="J11">
+        <v>0.1</v>
+      </c>
+      <c r="K11">
+        <v>0.1</v>
+      </c>
+      <c r="L11">
+        <v>0.1</v>
+      </c>
+      <c r="M11">
         <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6711,7 +6351,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6759,20 +6399,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="1"/>
+    <col min="13" max="13" width="16.88671875" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -6780,75 +6420,75 @@
   <sheetData>
     <row r="1" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>170</v>
+        <v>144</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>97</v>
       </c>
       <c r="N1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="O1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="P1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="18">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E2">
         <v>256</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H2">
         <v>19</v>
@@ -6865,40 +6505,40 @@
       <c r="L2">
         <v>48</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>183</v>
+      <c r="M2" s="19">
+        <v>111282</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>293</v>
+      <c r="B3">
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E3">
         <v>128</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H3">
         <v>19</v>
@@ -6915,40 +6555,40 @@
       <c r="L3">
         <v>48</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>184</v>
+      <c r="M3" s="19">
+        <v>170651</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E4">
         <v>256</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H4">
         <v>19</v>
@@ -6965,40 +6605,40 @@
       <c r="L4">
         <v>48</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>187</v>
+      <c r="M4" s="19">
+        <v>244723</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E5">
         <v>256</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H5">
         <v>19</v>
@@ -7015,40 +6655,40 @@
       <c r="L5">
         <v>82</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>188</v>
+      <c r="M5" s="19">
+        <v>94201</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E6">
         <v>64</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H6" s="2">
         <v>17</v>
@@ -7065,40 +6705,40 @@
       <c r="L6">
         <v>82</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>189</v>
+      <c r="M6" s="19">
+        <v>143162</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E7">
         <v>128</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H7">
         <v>19</v>
@@ -7115,40 +6755,40 @@
       <c r="L7">
         <v>84</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>191</v>
+      <c r="M7" s="19">
+        <v>76449</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8">
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E8">
         <v>256</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H8">
         <v>19</v>
@@ -7165,40 +6805,40 @@
       <c r="L8">
         <v>84</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>192</v>
+      <c r="M8" s="19">
+        <v>86756</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E9">
         <v>128</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H9" s="2">
         <v>17</v>
@@ -7215,40 +6855,40 @@
       <c r="L9">
         <v>83</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>193</v>
+      <c r="M9" s="19">
+        <v>128846</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E10">
         <v>128</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H10">
         <v>19</v>
@@ -7265,40 +6905,40 @@
       <c r="L10">
         <v>83.5</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>194</v>
+      <c r="M10" s="19">
+        <v>137436</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11">
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E11">
         <v>256</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H11" s="2">
         <v>17</v>
@@ -7315,40 +6955,40 @@
       <c r="L11">
         <v>84</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>195</v>
+      <c r="M11" s="19">
+        <v>138436</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12">
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E12">
         <v>256</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="H12">
         <v>19</v>
@@ -7365,17 +7005,17 @@
       <c r="L12">
         <v>82</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>196</v>
+      <c r="M12" s="19">
+        <v>148889</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -7388,8 +7028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7416,61 +7056,61 @@
   <sheetData>
     <row r="1" spans="1:19" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="Q1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="R1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="S1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
@@ -7519,7 +7159,7 @@
       <c r="O2" s="1">
         <v>400</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="15">
         <v>170528.88</v>
       </c>
       <c r="Q2">
@@ -7578,7 +7218,7 @@
       <c r="O3" s="1">
         <v>400</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <v>161857.84</v>
       </c>
       <c r="Q3">
@@ -7637,7 +7277,7 @@
       <c r="O4" s="1">
         <v>400</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="15">
         <v>233304.86</v>
       </c>
       <c r="Q4">
@@ -7652,7 +7292,7 @@
     </row>
     <row r="5" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B5">
         <v>3000</v>
@@ -7696,7 +7336,7 @@
       <c r="O5" s="1">
         <v>450</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="14">
         <v>673016</v>
       </c>
       <c r="Q5">
@@ -7711,7 +7351,7 @@
     </row>
     <row r="6" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="B6">
         <v>4000</v>
@@ -7755,7 +7395,7 @@
       <c r="O6" s="1">
         <v>450</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="14">
         <v>934812</v>
       </c>
       <c r="Q6">
@@ -7814,7 +7454,7 @@
       <c r="O7" s="4">
         <v>350</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <v>55547.42</v>
       </c>
       <c r="Q7">
@@ -7873,7 +7513,7 @@
       <c r="O8" s="4">
         <v>300</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="16">
         <v>14963.66</v>
       </c>
       <c r="Q8">
@@ -7932,7 +7572,7 @@
       <c r="O9" s="4">
         <v>350</v>
       </c>
-      <c r="P9" s="17">
+      <c r="P9" s="16">
         <v>32858.879999999997</v>
       </c>
       <c r="Q9" s="2">
@@ -7991,7 +7631,7 @@
       <c r="O10" s="4">
         <v>350</v>
       </c>
-      <c r="P10" s="17">
+      <c r="P10" s="16">
         <v>34054.230000000003</v>
       </c>
       <c r="Q10">
@@ -8006,66 +7646,66 @@
     </row>
     <row r="11" spans="1:19" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="F11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="H11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="J11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="K11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="L11" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="N11" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B12">
         <v>0.1</v>
@@ -8110,12 +7750,21 @@
         <v>0.1</v>
       </c>
       <c r="P12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S12" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B13">
         <v>5000</v>
@@ -8174,7 +7823,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -8244,7 +7893,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:Q13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8257,55 +7908,55 @@
   <sheetData>
     <row r="1" spans="1:17" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="O1" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="P1" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="Q1" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
@@ -8339,7 +7990,7 @@
       <c r="J2">
         <v>2</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <v>43.64</v>
       </c>
       <c r="L2">
@@ -8392,13 +8043,13 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="17">
         <v>16.36</v>
       </c>
       <c r="L3">
         <v>45</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="13">
         <v>45</v>
       </c>
       <c r="N3">
@@ -8445,7 +8096,7 @@
       <c r="J4">
         <v>2</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>21.36</v>
       </c>
       <c r="L4">
@@ -8495,10 +8146,10 @@
       <c r="I5">
         <v>5</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>0.5</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <v>10</v>
       </c>
       <c r="L5">
@@ -8548,10 +8199,10 @@
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>0.5</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>9.09</v>
       </c>
       <c r="L6">
@@ -8604,7 +8255,7 @@
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <v>11.36</v>
       </c>
       <c r="L7">
@@ -8657,7 +8308,7 @@
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="13">
         <v>10.77</v>
       </c>
       <c r="L8">
@@ -8710,7 +8361,7 @@
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <v>12.7</v>
       </c>
       <c r="L9">
@@ -8763,7 +8414,7 @@
       <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <v>11.34</v>
       </c>
       <c r="L10">
@@ -8816,7 +8467,7 @@
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <v>12.27</v>
       </c>
       <c r="L11">
@@ -8840,60 +8491,60 @@
     </row>
     <row r="12" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="F12" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="G12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="H12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="I12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="J12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="L12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="M12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="N12" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="B13">
         <v>0.1</v>
@@ -8932,12 +8583,21 @@
         <v>0.1</v>
       </c>
       <c r="N13">
+        <v>0.1</v>
+      </c>
+      <c r="O13">
+        <v>0.1</v>
+      </c>
+      <c r="P13">
+        <v>0.1</v>
+      </c>
+      <c r="Q13">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="B14">
         <v>5000</v>
@@ -8990,7 +8650,7 @@
     </row>
     <row r="15" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B15">
         <v>300</v>
@@ -9016,7 +8676,7 @@
       <c r="I15">
         <v>1</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <v>0.25</v>
       </c>
       <c r="K15">

</xml_diff>

<commit_message>
Changed criterion files. Rules are changed to match input data from excel
</commit_message>
<xml_diff>
--- a/Элементы СКС_для_Жени.xlsx
+++ b/Элементы СКС_для_Жени.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ВОЛС" sheetId="5" r:id="rId1"/>
@@ -392,9 +392,6 @@
     <t>Сплайс кассеты</t>
   </si>
   <si>
-    <t>АБС-пластик</t>
-  </si>
-  <si>
     <t>Черный</t>
   </si>
   <si>
@@ -807,6 +804,9 @@
   </si>
   <si>
     <t>Количество КДЗС</t>
+  </si>
+  <si>
+    <t>Пластик</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -907,6 +907,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1228,16 +1229,16 @@
         <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" t="s">
         <v>250</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>251</v>
-      </c>
-      <c r="J1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1562,39 +1563,39 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13">
         <v>0.05</v>
@@ -1626,7 +1627,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1658,7 +1659,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1714,37 +1715,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="66" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K1" t="s">
         <v>250</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>251</v>
-      </c>
-      <c r="L1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2167,45 +2168,45 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13" t="s">
+        <v>245</v>
+      </c>
+      <c r="F13" t="s">
+        <v>245</v>
+      </c>
+      <c r="G13" t="s">
+        <v>245</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C13" t="s">
+      <c r="I13" t="s">
         <v>246</v>
       </c>
-      <c r="D13" t="s">
-        <v>246</v>
-      </c>
-      <c r="E13" t="s">
-        <v>246</v>
-      </c>
-      <c r="F13" t="s">
-        <v>246</v>
-      </c>
-      <c r="G13" t="s">
-        <v>246</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I13" t="s">
-        <v>247</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B14">
         <v>0.1</v>
@@ -2243,7 +2244,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15">
         <v>100</v>
@@ -2281,7 +2282,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2345,49 +2346,49 @@
   <sheetData>
     <row r="1" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>207</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N1" t="s">
+        <v>249</v>
+      </c>
+      <c r="O1" t="s">
         <v>250</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>251</v>
-      </c>
-      <c r="P1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -2442,7 +2443,7 @@
     </row>
     <row r="3" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -2492,7 +2493,7 @@
     </row>
     <row r="4" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -2542,7 +2543,7 @@
     </row>
     <row r="5" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="12">
         <v>3</v>
@@ -2592,7 +2593,7 @@
     </row>
     <row r="6" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" s="12">
         <v>3</v>
@@ -2642,7 +2643,7 @@
     </row>
     <row r="7" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -2692,7 +2693,7 @@
     </row>
     <row r="8" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B8" s="12">
         <v>3</v>
@@ -2742,7 +2743,7 @@
     </row>
     <row r="9" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" s="12">
         <v>3</v>
@@ -2792,7 +2793,7 @@
     </row>
     <row r="10" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -2842,7 +2843,7 @@
     </row>
     <row r="11" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2892,57 +2893,57 @@
     </row>
     <row r="12" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="F12" t="s">
         <v>246</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>246</v>
       </c>
-      <c r="E12" t="s">
-        <v>247</v>
-      </c>
-      <c r="F12" t="s">
-        <v>247</v>
-      </c>
-      <c r="G12" t="s">
-        <v>247</v>
-      </c>
       <c r="H12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I12" t="s">
+        <v>245</v>
+      </c>
+      <c r="J12" t="s">
+        <v>245</v>
+      </c>
+      <c r="K12" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" t="s">
+        <v>245</v>
+      </c>
+      <c r="M12" t="s">
         <v>246</v>
       </c>
-      <c r="J12" t="s">
-        <v>246</v>
-      </c>
-      <c r="K12" t="s">
-        <v>246</v>
-      </c>
-      <c r="L12" t="s">
-        <v>246</v>
-      </c>
-      <c r="M12" t="s">
-        <v>247</v>
-      </c>
       <c r="N12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="1">
         <v>0.1</v>
@@ -2992,7 +2993,7 @@
     </row>
     <row r="14" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
@@ -3042,7 +3043,7 @@
     </row>
     <row r="15" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -3145,60 +3146,60 @@
   <sheetData>
     <row r="1" spans="1:18" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="H1" t="s">
-        <v>222</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P1" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q1" t="s">
         <v>250</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>251</v>
-      </c>
-      <c r="R1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -3254,7 +3255,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
@@ -3310,7 +3311,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -3366,7 +3367,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -3422,7 +3423,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -3478,7 +3479,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -3534,7 +3535,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -3590,7 +3591,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -3646,7 +3647,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -3702,7 +3703,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -3758,63 +3759,63 @@
     </row>
     <row r="12" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H12" t="s">
+        <v>245</v>
+      </c>
+      <c r="I12" t="s">
+        <v>245</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F12" t="s">
-        <v>246</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="H12" t="s">
-        <v>246</v>
-      </c>
-      <c r="I12" t="s">
-        <v>246</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="P12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" s="1">
         <v>0.1</v>
@@ -3870,7 +3871,7 @@
     </row>
     <row r="14" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
@@ -3926,7 +3927,7 @@
     </row>
     <row r="15" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -4015,28 +4016,28 @@
         <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
         <v>97</v>
       </c>
       <c r="I1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1" t="s">
         <v>250</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>251</v>
-      </c>
-      <c r="K1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4047,7 +4048,7 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
         <v>102</v>
@@ -4065,13 +4066,13 @@
         <v>800</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="66" x14ac:dyDescent="0.25">
@@ -4100,13 +4101,13 @@
         <v>1500</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="66" x14ac:dyDescent="0.25">
@@ -4135,13 +4136,13 @@
         <v>3100</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="66" x14ac:dyDescent="0.25">
@@ -4170,13 +4171,13 @@
         <v>2900</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4187,7 +4188,7 @@
         <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D6" t="s">
         <v>102</v>
@@ -4205,13 +4206,13 @@
         <v>1800</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4222,7 +4223,7 @@
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D7" t="s">
         <v>102</v>
@@ -4240,13 +4241,13 @@
         <v>2700</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4257,7 +4258,7 @@
         <v>113</v>
       </c>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D8" t="s">
         <v>102</v>
@@ -4275,13 +4276,13 @@
         <v>3500</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4292,7 +4293,7 @@
         <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
         <v>102</v>
@@ -4310,13 +4311,13 @@
         <v>1700</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4327,7 +4328,7 @@
         <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D10" t="s">
         <v>102</v>
@@ -4345,13 +4346,13 @@
         <v>2400</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
@@ -4362,7 +4363,7 @@
         <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" t="s">
         <v>102</v>
@@ -4380,13 +4381,13 @@
         <v>3100</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4432,16 +4433,16 @@
         <v>106</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" t="s">
         <v>250</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>251</v>
-      </c>
-      <c r="I1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="66" x14ac:dyDescent="0.25">
@@ -4649,36 +4650,36 @@
     </row>
     <row r="9" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" t="s">
         <v>246</v>
       </c>
-      <c r="C9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E9" t="s">
-        <v>246</v>
-      </c>
-      <c r="F9" t="s">
-        <v>247</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B10" s="2">
         <v>0.3</v>
@@ -4707,7 +4708,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
@@ -4736,7 +4737,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -4834,8 +4835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4854,7 +4855,7 @@
         <v>119</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>104</v>
@@ -4863,89 +4864,89 @@
         <v>106</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>103</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
         <v>249</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>250</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>251</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>150</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>150</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2">
-        <v>195</v>
-      </c>
-      <c r="F2">
-        <v>126</v>
-      </c>
-      <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2">
-        <v>100</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B3">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="E3">
         <v>195</v>
       </c>
       <c r="F3">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>254</v>
@@ -4955,35 +4956,35 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
+      <c r="A4" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B4">
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>258</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="E4">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="F4">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G4">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H4" s="2">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>253</v>
@@ -4991,69 +4992,69 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>258</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="E5">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
       <c r="G5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>258</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E6">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="F6">
-        <v>160</v>
+        <v>93</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2">
-        <v>420</v>
+        <v>125</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>253</v>
@@ -5061,69 +5062,69 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7">
+        <v>240</v>
+      </c>
+      <c r="F7">
         <v>120</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7">
-        <v>195</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
       <c r="G7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>120</v>
+        <v>258</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E8">
-        <v>110</v>
+        <v>234</v>
       </c>
       <c r="F8">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H8" s="2">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>254</v>
@@ -5131,63 +5132,63 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="F9">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="G9">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H9" s="2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>252</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E10">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="F10">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H10" s="2">
-        <v>140</v>
+        <v>300</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>254</v>
@@ -5201,28 +5202,28 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B11">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E11">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F11">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="G11">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H11" s="2">
-        <v>120</v>
+        <v>420</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>254</v>
@@ -5231,11 +5232,12 @@
         <v>253</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5244,7 +5246,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:O10"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5266,49 +5268,49 @@
   <sheetData>
     <row r="1" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>97</v>
       </c>
       <c r="M1" t="s">
+        <v>249</v>
+      </c>
+      <c r="N1" t="s">
         <v>250</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>251</v>
-      </c>
-      <c r="O1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="118.8" x14ac:dyDescent="0.25">
@@ -5548,7 +5550,7 @@
     </row>
     <row r="7" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5642,54 +5644,54 @@
     </row>
     <row r="9" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" t="s">
         <v>246</v>
       </c>
-      <c r="C9" t="s">
+      <c r="H9" t="s">
         <v>246</v>
       </c>
-      <c r="D9" t="s">
+      <c r="I9" t="s">
         <v>246</v>
       </c>
-      <c r="E9" t="s">
+      <c r="J9" t="s">
         <v>246</v>
       </c>
-      <c r="F9" t="s">
+      <c r="K9" t="s">
+        <v>245</v>
+      </c>
+      <c r="L9" t="s">
         <v>246</v>
       </c>
-      <c r="G9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H9" t="s">
-        <v>247</v>
-      </c>
-      <c r="I9" t="s">
-        <v>247</v>
-      </c>
-      <c r="J9" t="s">
-        <v>247</v>
-      </c>
-      <c r="K9" t="s">
-        <v>246</v>
-      </c>
-      <c r="L9" t="s">
-        <v>247</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B10">
         <v>0.05</v>
@@ -5736,7 +5738,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -5783,7 +5785,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -5859,43 +5861,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
         <v>136</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>139</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>140</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>141</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>142</v>
-      </c>
-      <c r="I1" t="s">
-        <v>143</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>97</v>
       </c>
       <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
         <v>250</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>251</v>
-      </c>
-      <c r="M1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="79.2" x14ac:dyDescent="0.25">
@@ -6228,48 +6230,48 @@
     </row>
     <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" t="s">
         <v>246</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
+        <v>245</v>
+      </c>
+      <c r="H10" t="s">
+        <v>245</v>
+      </c>
+      <c r="I10" t="s">
+        <v>245</v>
+      </c>
+      <c r="J10" t="s">
         <v>246</v>
       </c>
-      <c r="D10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E10" t="s">
-        <v>246</v>
-      </c>
-      <c r="F10" t="s">
-        <v>247</v>
-      </c>
-      <c r="G10" t="s">
-        <v>246</v>
-      </c>
-      <c r="H10" t="s">
-        <v>246</v>
-      </c>
-      <c r="I10" t="s">
-        <v>246</v>
-      </c>
-      <c r="J10" t="s">
-        <v>247</v>
-      </c>
       <c r="K10" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -6310,7 +6312,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6351,7 +6353,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -6399,8 +6401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6420,52 +6422,52 @@
   <sheetData>
     <row r="1" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>97</v>
       </c>
       <c r="N1" t="s">
+        <v>249</v>
+      </c>
+      <c r="O1" t="s">
         <v>250</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>251</v>
-      </c>
-      <c r="P1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
@@ -6476,46 +6478,46 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I2">
-        <v>15.35</v>
+        <v>18</v>
       </c>
       <c r="J2">
         <v>70.12</v>
       </c>
       <c r="K2">
-        <v>4.4000000000000004</v>
+        <v>14</v>
       </c>
       <c r="L2">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="M2" s="19">
-        <v>111282</v>
+        <v>171282</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>254</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="79.2" x14ac:dyDescent="0.25">
@@ -6526,19 +6528,19 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3">
         <v>128</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H3">
         <v>19</v>
@@ -6559,13 +6561,13 @@
         <v>170651</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="79.2" x14ac:dyDescent="0.25">
@@ -6576,19 +6578,19 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4">
         <v>256</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4">
         <v>19</v>
@@ -6609,13 +6611,13 @@
         <v>244723</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6626,19 +6628,19 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5">
         <v>256</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5">
         <v>19</v>
@@ -6659,13 +6661,13 @@
         <v>94201</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6676,19 +6678,19 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E6">
         <v>64</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H6" s="2">
         <v>17</v>
@@ -6709,13 +6711,13 @@
         <v>143162</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6726,19 +6728,19 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7">
         <v>128</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H7">
         <v>19</v>
@@ -6759,13 +6761,13 @@
         <v>76449</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6776,19 +6778,19 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8">
         <v>256</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H8">
         <v>19</v>
@@ -6809,13 +6811,13 @@
         <v>86756</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6826,19 +6828,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9">
         <v>128</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9" s="2">
         <v>17</v>
@@ -6859,13 +6861,13 @@
         <v>128846</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6876,19 +6878,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E10">
         <v>128</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H10">
         <v>19</v>
@@ -6909,13 +6911,13 @@
         <v>137436</v>
       </c>
       <c r="N10" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6926,19 +6928,19 @@
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11">
         <v>256</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H11" s="2">
         <v>17</v>
@@ -6959,13 +6961,13 @@
         <v>138436</v>
       </c>
       <c r="N11" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="P11" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
@@ -6976,19 +6978,19 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E12">
         <v>256</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H12">
         <v>19</v>
@@ -7009,13 +7011,13 @@
         <v>148889</v>
       </c>
       <c r="N12" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="P12" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -7056,61 +7058,61 @@
   <sheetData>
     <row r="1" spans="1:19" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="Q1" t="s">
+        <v>249</v>
+      </c>
+      <c r="R1" t="s">
         <v>250</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>251</v>
-      </c>
-      <c r="S1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
@@ -7292,7 +7294,7 @@
     </row>
     <row r="5" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5">
         <v>3000</v>
@@ -7351,7 +7353,7 @@
     </row>
     <row r="6" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6">
         <v>4000</v>
@@ -7646,66 +7648,66 @@
     </row>
     <row r="11" spans="1:19" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G11" t="s">
+        <v>245</v>
+      </c>
+      <c r="H11" t="s">
+        <v>245</v>
+      </c>
+      <c r="I11" t="s">
+        <v>245</v>
+      </c>
+      <c r="J11" t="s">
+        <v>245</v>
+      </c>
+      <c r="K11" t="s">
+        <v>245</v>
+      </c>
+      <c r="L11" t="s">
+        <v>245</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N11" t="s">
         <v>246</v>
       </c>
-      <c r="C11" t="s">
+      <c r="O11" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F11" t="s">
-        <v>246</v>
-      </c>
-      <c r="G11" t="s">
-        <v>246</v>
-      </c>
-      <c r="H11" t="s">
-        <v>246</v>
-      </c>
-      <c r="I11" t="s">
-        <v>246</v>
-      </c>
-      <c r="J11" t="s">
-        <v>246</v>
-      </c>
-      <c r="K11" t="s">
-        <v>246</v>
-      </c>
-      <c r="L11" t="s">
-        <v>246</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="N11" t="s">
-        <v>247</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="Q11" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B12">
         <v>0.1</v>
@@ -7764,7 +7766,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13">
         <v>5000</v>
@@ -7823,7 +7825,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -7908,55 +7910,55 @@
   <sheetData>
     <row r="1" spans="1:17" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="O1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P1" t="s">
         <v>250</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>251</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
@@ -8491,60 +8493,60 @@
     </row>
     <row r="12" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G12" t="s">
         <v>246</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H12" t="s">
         <v>246</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>246</v>
       </c>
-      <c r="G12" t="s">
-        <v>247</v>
-      </c>
-      <c r="H12" t="s">
-        <v>247</v>
-      </c>
-      <c r="I12" t="s">
-        <v>247</v>
-      </c>
       <c r="J12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13">
         <v>0.1</v>
@@ -8597,7 +8599,7 @@
     </row>
     <row r="14" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14">
         <v>5000</v>
@@ -8650,7 +8652,7 @@
     </row>
     <row r="15" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15">
         <v>300</v>

</xml_diff>